<commit_message>
Local awareness for sorted() added
</commit_message>
<xml_diff>
--- a/Рознарядка.xlsx
+++ b/Рознарядка.xlsx
@@ -32123,44 +32123,44 @@
       </c>
       <c r="B3" s="27" t="inlineStr">
         <is>
-          <t>Богородчанське ЛВУМГ</t>
+          <t>Бібрське ЛВУМГ</t>
         </is>
       </c>
       <c r="C3" s="27" t="n">
-        <v>11.47</v>
+        <v>11.656</v>
       </c>
       <c r="D3" s="27" t="n">
-        <v>5452</v>
+        <v>2474</v>
       </c>
       <c r="E3" s="27" t="n">
-        <v>0.579</v>
+        <v>0.8860000000000001</v>
       </c>
       <c r="F3" s="27" t="n"/>
       <c r="G3" s="27" t="n">
-        <v>4.543</v>
+        <v>2.506</v>
       </c>
       <c r="H3" s="27" t="n">
-        <v>0.836</v>
+        <v>0.9690000000000001</v>
       </c>
       <c r="I3" s="27" t="n">
-        <v>0.23</v>
+        <v>0.295</v>
       </c>
       <c r="J3" s="27" t="n"/>
       <c r="K3" s="27" t="n"/>
       <c r="L3" s="27" t="n">
-        <v>1.448</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="M3" s="27" t="n">
-        <v>1.796</v>
+        <v>1.369</v>
       </c>
       <c r="N3" s="27" t="n">
-        <v>3041</v>
+        <v>2557</v>
       </c>
       <c r="O3" s="27" t="n">
-        <v>1789</v>
+        <v>742</v>
       </c>
       <c r="P3" s="27" t="n">
-        <v>4.02</v>
+        <v>3.756</v>
       </c>
     </row>
     <row r="4">
@@ -32169,44 +32169,44 @@
       </c>
       <c r="B4" s="27" t="inlineStr">
         <is>
-          <t>Богородчанське ЛВУМГ (Долинське)</t>
+          <t>Бібрське ЛВУМГ (Рівненське)</t>
         </is>
       </c>
       <c r="C4" s="27" t="n">
-        <v>6.42</v>
+        <v>11.681</v>
       </c>
       <c r="D4" s="27" t="n">
-        <v>2084</v>
+        <v>2134</v>
       </c>
       <c r="E4" s="27" t="n">
-        <v>0.105</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F4" s="27" t="n"/>
       <c r="G4" s="27" t="n">
-        <v>2.164</v>
+        <v>2.118</v>
       </c>
       <c r="H4" s="27" t="n">
-        <v>0.536</v>
+        <v>1.869</v>
       </c>
       <c r="I4" s="27" t="n">
-        <v>0.226</v>
+        <v>0.263</v>
       </c>
       <c r="J4" s="27" t="n"/>
       <c r="K4" s="27" t="n"/>
       <c r="L4" s="27" t="n">
-        <v>0.4950000000000001</v>
+        <v>4.642999999999999</v>
       </c>
       <c r="M4" s="27" t="n">
-        <v>0.6930000000000001</v>
+        <v>1.214</v>
       </c>
       <c r="N4" s="27" t="n">
-        <v>1412</v>
+        <v>2442.097</v>
       </c>
       <c r="O4" s="27" t="n">
-        <v>500</v>
+        <v>1104</v>
       </c>
       <c r="P4" s="27" t="n">
-        <v>2.374</v>
+        <v>3.892</v>
       </c>
     </row>
     <row r="5">
@@ -32215,44 +32215,44 @@
       </c>
       <c r="B5" s="27" t="inlineStr">
         <is>
-          <t>Боярське ЛВУМГ</t>
+          <t>Богородчанське ЛВУМГ</t>
         </is>
       </c>
       <c r="C5" s="27" t="n">
-        <v>14.367</v>
+        <v>11.47</v>
       </c>
       <c r="D5" s="27" t="n">
-        <v>4676</v>
+        <v>5452</v>
       </c>
       <c r="E5" s="27" t="n">
-        <v>1.18</v>
+        <v>0.579</v>
       </c>
       <c r="F5" s="27" t="n"/>
       <c r="G5" s="27" t="n">
-        <v>4.721</v>
+        <v>4.543</v>
       </c>
       <c r="H5" s="27" t="n">
-        <v>1.36</v>
+        <v>0.836</v>
       </c>
       <c r="I5" s="27" t="n">
-        <v>0.47</v>
+        <v>0.23</v>
       </c>
       <c r="J5" s="27" t="n"/>
       <c r="K5" s="27" t="n"/>
       <c r="L5" s="27" t="n">
-        <v>1.478</v>
+        <v>1.448</v>
       </c>
       <c r="M5" s="27" t="n">
-        <v>2.601</v>
+        <v>1.796</v>
       </c>
       <c r="N5" s="27" t="n">
-        <v>4393</v>
+        <v>3041</v>
       </c>
       <c r="O5" s="27" t="n">
-        <v>1792.07</v>
+        <v>1789</v>
       </c>
       <c r="P5" s="27" t="n">
-        <v>6.631</v>
+        <v>4.02</v>
       </c>
     </row>
     <row r="6">
@@ -32261,44 +32261,44 @@
       </c>
       <c r="B6" s="27" t="inlineStr">
         <is>
-          <t>Бібрське ЛВУМГ</t>
+          <t>Богородчанське ЛВУМГ (Долинське)</t>
         </is>
       </c>
       <c r="C6" s="27" t="n">
-        <v>11.656</v>
+        <v>6.42</v>
       </c>
       <c r="D6" s="27" t="n">
-        <v>2474</v>
+        <v>2084</v>
       </c>
       <c r="E6" s="27" t="n">
-        <v>0.8860000000000001</v>
+        <v>0.105</v>
       </c>
       <c r="F6" s="27" t="n"/>
       <c r="G6" s="27" t="n">
-        <v>2.506</v>
+        <v>2.164</v>
       </c>
       <c r="H6" s="27" t="n">
-        <v>0.9690000000000001</v>
+        <v>0.536</v>
       </c>
       <c r="I6" s="27" t="n">
-        <v>0.295</v>
+        <v>0.226</v>
       </c>
       <c r="J6" s="27" t="n"/>
       <c r="K6" s="27" t="n"/>
       <c r="L6" s="27" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.4950000000000001</v>
       </c>
       <c r="M6" s="27" t="n">
-        <v>1.369</v>
+        <v>0.6930000000000001</v>
       </c>
       <c r="N6" s="27" t="n">
-        <v>2557</v>
+        <v>1412</v>
       </c>
       <c r="O6" s="27" t="n">
-        <v>742</v>
+        <v>500</v>
       </c>
       <c r="P6" s="27" t="n">
-        <v>3.756</v>
+        <v>2.374</v>
       </c>
     </row>
     <row r="7">
@@ -32307,44 +32307,44 @@
       </c>
       <c r="B7" s="27" t="inlineStr">
         <is>
-          <t>Бібрське ЛВУМГ (Рівненське)</t>
+          <t>Боярське ЛВУМГ</t>
         </is>
       </c>
       <c r="C7" s="27" t="n">
-        <v>11.681</v>
+        <v>14.367</v>
       </c>
       <c r="D7" s="27" t="n">
-        <v>2134</v>
+        <v>4676</v>
       </c>
       <c r="E7" s="27" t="n">
-        <v>0.5600000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="F7" s="27" t="n"/>
       <c r="G7" s="27" t="n">
-        <v>2.118</v>
+        <v>4.721</v>
       </c>
       <c r="H7" s="27" t="n">
-        <v>1.869</v>
+        <v>1.36</v>
       </c>
       <c r="I7" s="27" t="n">
-        <v>0.263</v>
+        <v>0.47</v>
       </c>
       <c r="J7" s="27" t="n"/>
       <c r="K7" s="27" t="n"/>
       <c r="L7" s="27" t="n">
-        <v>4.642999999999999</v>
+        <v>1.478</v>
       </c>
       <c r="M7" s="27" t="n">
-        <v>1.214</v>
+        <v>2.601</v>
       </c>
       <c r="N7" s="27" t="n">
-        <v>2442.097</v>
+        <v>4393</v>
       </c>
       <c r="O7" s="27" t="n">
-        <v>1104</v>
+        <v>1792.07</v>
       </c>
       <c r="P7" s="27" t="n">
-        <v>3.892</v>
+        <v>6.631</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Added units to distribution_ws
</commit_message>
<xml_diff>
--- a/Рознарядка.xlsx
+++ b/Рознарядка.xlsx
@@ -84,7 +84,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -237,6 +237,39 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -634,7 +667,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -755,7 +788,7 @@
       <c r="N4" s="12" t="n"/>
       <c r="O4" s="7" t="inlineStr">
         <is>
-          <t>v</t>
+          <t>км</t>
         </is>
       </c>
       <c r="P4" s="3" t="n">
@@ -885,7 +918,11 @@
       <c r="L8" s="11" t="n"/>
       <c r="M8" s="11" t="n"/>
       <c r="N8" s="12" t="n"/>
-      <c r="O8" s="7" t="n"/>
+      <c r="O8" s="7" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
       <c r="P8" s="6" t="n">
         <v>18.222</v>
       </c>
@@ -31890,7 +31927,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31956,886 +31993,964 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>Бердичівське ЛВУМГ</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>12.245</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>1908</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="n">
-        <v>5.394</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>1.051</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>0.303</v>
-      </c>
-      <c r="J2" s="2" t="n"/>
-      <c r="K2" s="2" t="n"/>
-      <c r="L2" s="2" t="n">
-        <v>0.716</v>
-      </c>
-      <c r="M2" s="2" t="n">
-        <v>1.214</v>
-      </c>
-      <c r="N2" s="2" t="n">
-        <v>2523</v>
-      </c>
-      <c r="O2" s="2" t="n">
-        <v>1168</v>
-      </c>
-      <c r="P2" s="2" t="n">
-        <v>3.52</v>
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="M2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
+          <t>км</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Бібрське ЛВУМГ</t>
+          <t>Бердичівське ЛВУМГ</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>11.656</v>
+        <v>12.245</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>2474</v>
+        <v>1908</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.8860000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="F3" s="2" t="n"/>
       <c r="G3" s="2" t="n">
-        <v>2.506</v>
+        <v>5.394</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>0.9690000000000001</v>
+        <v>1.051</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>0.295</v>
+        <v>0.303</v>
       </c>
       <c r="J3" s="2" t="n"/>
       <c r="K3" s="2" t="n"/>
       <c r="L3" s="2" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.716</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>1.369</v>
+        <v>1.214</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>2557</v>
+        <v>2523</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>742</v>
+        <v>1168</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>3.756</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Бібрське ЛВУМГ (Рівненське)</t>
+          <t>Бібрське ЛВУМГ</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>11.681</v>
+        <v>11.656</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2134</v>
+        <v>2474</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.8860000000000001</v>
       </c>
       <c r="F4" s="2" t="n"/>
       <c r="G4" s="2" t="n">
-        <v>2.118</v>
+        <v>2.506</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>1.869</v>
+        <v>0.9690000000000001</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>0.263</v>
+        <v>0.295</v>
       </c>
       <c r="J4" s="2" t="n"/>
       <c r="K4" s="2" t="n"/>
       <c r="L4" s="2" t="n">
-        <v>4.642999999999999</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>1.214</v>
+        <v>1.369</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>2442.097</v>
+        <v>2557</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>1104</v>
+        <v>742</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>3.892</v>
+        <v>3.756</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>Богородчанське ЛВУМГ</t>
+          <t>Бібрське ЛВУМГ (Рівненське)</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>11.47</v>
+        <v>11.681</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>5452</v>
+        <v>2134</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.579</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F5" s="2" t="n"/>
       <c r="G5" s="2" t="n">
-        <v>4.543</v>
+        <v>2.118</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>0.836</v>
+        <v>1.869</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>0.23</v>
+        <v>0.263</v>
       </c>
       <c r="J5" s="2" t="n"/>
       <c r="K5" s="2" t="n"/>
       <c r="L5" s="2" t="n">
-        <v>1.448</v>
+        <v>4.642999999999999</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>1.796</v>
+        <v>1.214</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>3041</v>
+        <v>2442.097</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>1789</v>
+        <v>1104</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>4.02</v>
+        <v>3.892</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>Богородчанське ЛВУМГ (Долинське)</t>
+          <t>Богородчанське ЛВУМГ</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>6.42</v>
+        <v>11.47</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>2084</v>
+        <v>5452</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0.105</v>
+        <v>0.579</v>
       </c>
       <c r="F6" s="2" t="n"/>
       <c r="G6" s="2" t="n">
-        <v>2.164</v>
+        <v>4.543</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>0.536</v>
+        <v>0.836</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>0.226</v>
+        <v>0.23</v>
       </c>
       <c r="J6" s="2" t="n"/>
       <c r="K6" s="2" t="n"/>
       <c r="L6" s="2" t="n">
-        <v>0.4950000000000001</v>
+        <v>1.448</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>0.6930000000000001</v>
+        <v>1.796</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>1412</v>
+        <v>3041</v>
       </c>
       <c r="O6" s="2" t="n">
-        <v>500</v>
+        <v>1789</v>
       </c>
       <c r="P6" s="2" t="n">
-        <v>2.374</v>
+        <v>4.02</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>Боярське ЛВУМГ</t>
+          <t>Богородчанське ЛВУМГ (Долинське)</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>14.367</v>
+        <v>6.42</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>4676</v>
+        <v>2084</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>1.18</v>
+        <v>0.105</v>
       </c>
       <c r="F7" s="2" t="n"/>
       <c r="G7" s="2" t="n">
-        <v>4.721</v>
+        <v>2.164</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>1.36</v>
+        <v>0.536</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>0.47</v>
+        <v>0.226</v>
       </c>
       <c r="J7" s="2" t="n"/>
       <c r="K7" s="2" t="n"/>
       <c r="L7" s="2" t="n">
-        <v>1.478</v>
+        <v>0.4950000000000001</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>2.601</v>
+        <v>0.6930000000000001</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>4393</v>
+        <v>1412</v>
       </c>
       <c r="O7" s="2" t="n">
-        <v>1792.07</v>
+        <v>500</v>
       </c>
       <c r="P7" s="2" t="n">
-        <v>6.631</v>
+        <v>2.374</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>Закарпатське ЛВУМГ</t>
+          <t>Боярське ЛВУМГ</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>7.121</v>
+        <v>14.367</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>2571</v>
+        <v>4676</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.773</v>
+        <v>1.18</v>
       </c>
       <c r="F8" s="2" t="n"/>
       <c r="G8" s="2" t="n">
-        <v>3.555</v>
+        <v>4.721</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>0.258</v>
+        <v>1.36</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.47</v>
       </c>
       <c r="J8" s="2" t="n"/>
       <c r="K8" s="2" t="n"/>
       <c r="L8" s="2" t="n">
-        <v>0.8160000000000001</v>
+        <v>1.478</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>0.6919999999999999</v>
+        <v>2.601</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>1711</v>
+        <v>4393</v>
       </c>
       <c r="O8" s="2" t="n">
-        <v>1149</v>
+        <v>1792.07</v>
       </c>
       <c r="P8" s="2" t="n">
-        <v>3.724</v>
+        <v>6.631</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>Запорізьке ЛВУМГ</t>
+          <t>Закарпатське ЛВУМГ</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>8.911</v>
+        <v>7.121</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>1800</v>
+        <v>2571</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>1.395</v>
+        <v>0.773</v>
       </c>
       <c r="F9" s="2" t="n"/>
       <c r="G9" s="2" t="n">
-        <v>2.293</v>
+        <v>3.555</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>1.422</v>
+        <v>0.258</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>0.378</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="J9" s="2" t="n"/>
       <c r="K9" s="2" t="n"/>
       <c r="L9" s="2" t="n">
-        <v>1.127</v>
+        <v>0.8160000000000001</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>1.115</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="N9" s="2" t="n">
-        <v>2658</v>
+        <v>1711</v>
       </c>
       <c r="O9" s="2" t="n">
-        <v>925</v>
+        <v>1149</v>
       </c>
       <c r="P9" s="2" t="n">
-        <v>3.175</v>
+        <v>3.724</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>Запорізьке ЛВУМГ (Криворізьке)</t>
+          <t>Запорізьке ЛВУМГ</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>10.33</v>
+        <v>8.911</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>1774</v>
-      </c>
-      <c r="E10" s="2" t="n"/>
+        <v>1800</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>1.395</v>
+      </c>
       <c r="F10" s="2" t="n"/>
       <c r="G10" s="2" t="n">
-        <v>2.05</v>
+        <v>2.293</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0.417</v>
+        <v>1.422</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>0.162</v>
+        <v>0.378</v>
       </c>
       <c r="J10" s="2" t="n"/>
       <c r="K10" s="2" t="n"/>
       <c r="L10" s="2" t="n">
-        <v>1.035</v>
+        <v>1.127</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0.64</v>
+        <v>1.115</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>2157</v>
+        <v>2658</v>
       </c>
       <c r="O10" s="2" t="n">
-        <v>1150</v>
+        <v>925</v>
       </c>
       <c r="P10" s="2" t="n">
-        <v>2.624</v>
+        <v>3.175</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>Золотоніське ЛВУМГ</t>
+          <t>Запорізьке ЛВУМГ (Криворізьке)</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>8.470000000000001</v>
+        <v>10.33</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>1697</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0.9199999999999999</v>
-      </c>
+        <v>1774</v>
+      </c>
+      <c r="E11" s="2" t="n"/>
       <c r="F11" s="2" t="n"/>
       <c r="G11" s="2" t="n">
-        <v>20.687</v>
+        <v>2.05</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>0.449</v>
+        <v>0.417</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0.518</v>
-      </c>
-      <c r="J11" s="2" t="n">
-        <v>642</v>
-      </c>
+        <v>0.162</v>
+      </c>
+      <c r="J11" s="2" t="n"/>
       <c r="K11" s="2" t="n"/>
       <c r="L11" s="2" t="n">
-        <v>1.269</v>
+        <v>1.035</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0.876</v>
+        <v>0.64</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>2495</v>
+        <v>2157</v>
       </c>
       <c r="O11" s="2" t="n">
-        <v>1036</v>
+        <v>1150</v>
       </c>
       <c r="P11" s="2" t="n">
-        <v>2.96</v>
+        <v>2.624</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>Золотоніське ЛВУМГ (Барське)</t>
+          <t>Золотоніське ЛВУМГ</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>9.905000000000001</v>
+        <v>8.470000000000001</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>3681</v>
+        <v>1697</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>3.149</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>3.022</v>
-      </c>
+        <v>0.9199999999999999</v>
+      </c>
+      <c r="F12" s="2" t="n"/>
       <c r="G12" s="2" t="n">
-        <v>46.934</v>
+        <v>20.687</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>1.478</v>
+        <v>0.449</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>0.6500000000000001</v>
+        <v>0.518</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>612</v>
+        <v>642</v>
       </c>
       <c r="K12" s="2" t="n"/>
       <c r="L12" s="2" t="n">
-        <v>1.131</v>
+        <v>1.269</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>1.099</v>
+        <v>0.876</v>
       </c>
       <c r="N12" s="2" t="n">
-        <v>2124</v>
+        <v>2495</v>
       </c>
       <c r="O12" s="2" t="n">
-        <v>1460</v>
+        <v>1036</v>
       </c>
       <c r="P12" s="2" t="n">
-        <v>2.974999999999999</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>Краматорське ЛВУМГ</t>
+          <t>Золотоніське ЛВУМГ (Барське)</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>10.114</v>
+        <v>9.905000000000001</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>3324</v>
-      </c>
-      <c r="E13" s="2" t="n"/>
-      <c r="F13" s="2" t="n"/>
+        <v>3681</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>3.149</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>3.022</v>
+      </c>
       <c r="G13" s="2" t="n">
-        <v>4.485</v>
+        <v>46.934</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>1.208</v>
+        <v>1.478</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="J13" s="2" t="n"/>
+        <v>0.6500000000000001</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>612</v>
+      </c>
       <c r="K13" s="2" t="n"/>
       <c r="L13" s="2" t="n">
-        <v>0.904</v>
+        <v>1.131</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>0.863</v>
+        <v>1.099</v>
       </c>
       <c r="N13" s="2" t="n">
-        <v>2730</v>
+        <v>2124</v>
       </c>
       <c r="O13" s="2" t="n">
-        <v>1019</v>
+        <v>1460</v>
       </c>
       <c r="P13" s="2" t="n">
-        <v>4.949</v>
+        <v>2.974999999999999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>Краматорське ЛВУМГ (Сєвєродонецьке)</t>
+          <t>Краматорське ЛВУМГ</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>9.460000000000001</v>
+        <v>10.114</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>2277</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0.067</v>
-      </c>
+        <v>3324</v>
+      </c>
+      <c r="E14" s="2" t="n"/>
       <c r="F14" s="2" t="n"/>
       <c r="G14" s="2" t="n">
-        <v>3.296</v>
+        <v>4.485</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>0.519</v>
+        <v>1.208</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>0.174</v>
+        <v>0.33</v>
       </c>
       <c r="J14" s="2" t="n"/>
-      <c r="K14" s="2" t="n">
-        <v>0.7</v>
-      </c>
+      <c r="K14" s="2" t="n"/>
       <c r="L14" s="2" t="n">
-        <v>0.981</v>
+        <v>0.904</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>0.626</v>
+        <v>0.863</v>
       </c>
       <c r="N14" s="2" t="n">
-        <v>1955</v>
+        <v>2730</v>
       </c>
       <c r="O14" s="2" t="n">
-        <v>920</v>
+        <v>1019</v>
       </c>
       <c r="P14" s="2" t="n">
-        <v>3.368</v>
+        <v>4.949</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>Кременчуцьке ЛВУМГ</t>
+          <t>Краматорське ЛВУМГ (Сєвєродонецьке)</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>5.662</v>
+        <v>9.460000000000001</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>1066</v>
+        <v>2277</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>0.391</v>
+        <v>0.067</v>
       </c>
       <c r="F15" s="2" t="n"/>
       <c r="G15" s="2" t="n">
-        <v>6.476999999999999</v>
+        <v>3.296</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>0.115</v>
+        <v>0.519</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>0.482</v>
+        <v>0.174</v>
       </c>
       <c r="J15" s="2" t="n"/>
-      <c r="K15" s="2" t="n"/>
+      <c r="K15" s="2" t="n">
+        <v>0.7</v>
+      </c>
       <c r="L15" s="2" t="n">
-        <v>0.434</v>
+        <v>0.981</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>0.6639999999999999</v>
+        <v>0.626</v>
       </c>
       <c r="N15" s="2" t="n">
-        <v>1347</v>
+        <v>1955</v>
       </c>
       <c r="O15" s="2" t="n">
-        <v>1113</v>
+        <v>920</v>
       </c>
       <c r="P15" s="2" t="n">
-        <v>1.822</v>
+        <v>3.368</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>Лубенське ЛВУМГ</t>
+          <t>Кременчуцьке ЛВУМГ</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>16.756</v>
+        <v>5.662</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2475</v>
+        <v>1066</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="F16" s="2" t="n">
-        <v>0.2</v>
-      </c>
+        <v>0.391</v>
+      </c>
+      <c r="F16" s="2" t="n"/>
       <c r="G16" s="2" t="n">
-        <v>2.613</v>
+        <v>6.476999999999999</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>3.009</v>
+        <v>0.115</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>0.3119999999999999</v>
+        <v>0.482</v>
       </c>
       <c r="J16" s="2" t="n"/>
       <c r="K16" s="2" t="n"/>
       <c r="L16" s="2" t="n">
-        <v>2.092</v>
+        <v>0.434</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>1.622</v>
+        <v>0.6639999999999999</v>
       </c>
       <c r="N16" s="2" t="n">
-        <v>2848</v>
+        <v>1347</v>
       </c>
       <c r="O16" s="2" t="n">
-        <v>1262</v>
+        <v>1113</v>
       </c>
       <c r="P16" s="2" t="n">
-        <v>4.338</v>
+        <v>1.822</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>Миколаївське ЛВУМГ</t>
+          <t>Лубенське ЛВУМГ</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>16.943</v>
+        <v>16.756</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>3636</v>
+        <v>2475</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="F17" s="2" t="n"/>
+        <v>0.59</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>0.2</v>
+      </c>
       <c r="G17" s="2" t="n">
-        <v>4.725</v>
+        <v>2.613</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>1.04</v>
+        <v>3.009</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>0.288</v>
+        <v>0.3119999999999999</v>
       </c>
       <c r="J17" s="2" t="n"/>
       <c r="K17" s="2" t="n"/>
       <c r="L17" s="2" t="n">
-        <v>0.8300000000000001</v>
+        <v>2.092</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>2.111</v>
+        <v>1.622</v>
       </c>
       <c r="N17" s="2" t="n">
-        <v>4154</v>
+        <v>2848</v>
       </c>
       <c r="O17" s="2" t="n">
-        <v>2404</v>
+        <v>1262</v>
       </c>
       <c r="P17" s="2" t="n">
-        <v>4.45</v>
+        <v>4.338</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>Миколаївське ЛВУМГ(Одеське)</t>
+          <t>Миколаївське ЛВУМГ</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>15.1</v>
+        <v>16.943</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>3590</v>
+        <v>3636</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>5.62</v>
-      </c>
+        <v>0.12</v>
+      </c>
+      <c r="F18" s="2" t="n"/>
       <c r="G18" s="2" t="n">
-        <v>8.1</v>
+        <v>4.725</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>0.6</v>
+        <v>1.04</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>0.35</v>
+        <v>0.288</v>
       </c>
       <c r="J18" s="2" t="n"/>
       <c r="K18" s="2" t="n"/>
       <c r="L18" s="2" t="n">
-        <v>1.25</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>1.1</v>
+        <v>2.111</v>
       </c>
       <c r="N18" s="2" t="n">
-        <v>2749</v>
+        <v>4154</v>
       </c>
       <c r="O18" s="2" t="n">
-        <v>1113</v>
+        <v>2404</v>
       </c>
       <c r="P18" s="2" t="n">
-        <v>4.18</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>Сумське ЛВУМГ</t>
+          <t>Миколаївське ЛВУМГ(Одеське)</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>5.616</v>
+        <v>15.1</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>898</v>
-      </c>
-      <c r="E19" s="2" t="n"/>
-      <c r="F19" s="2" t="n"/>
+        <v>3590</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>5.62</v>
+      </c>
       <c r="G19" s="2" t="n">
-        <v>0.898</v>
+        <v>8.1</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>0.476</v>
+        <v>0.6</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>0.141</v>
+        <v>0.35</v>
       </c>
       <c r="J19" s="2" t="n"/>
       <c r="K19" s="2" t="n"/>
       <c r="L19" s="2" t="n">
-        <v>0.527</v>
+        <v>1.25</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>0.878</v>
+        <v>1.1</v>
       </c>
       <c r="N19" s="2" t="n">
-        <v>1289</v>
+        <v>2749</v>
       </c>
       <c r="O19" s="2" t="n">
-        <v>443</v>
+        <v>1113</v>
       </c>
       <c r="P19" s="2" t="n">
-        <v>1.611</v>
+        <v>4.18</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>Харківське ЛВУМГ</t>
+          <t>Сумське ЛВУМГ</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>9.907</v>
+        <v>5.616</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>2831</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>0.175</v>
-      </c>
+        <v>898</v>
+      </c>
+      <c r="E20" s="2" t="n"/>
       <c r="F20" s="2" t="n"/>
       <c r="G20" s="2" t="n">
-        <v>8.192</v>
+        <v>0.898</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>0.61</v>
+        <v>0.476</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>0.203</v>
+        <v>0.141</v>
       </c>
       <c r="J20" s="2" t="n"/>
       <c r="K20" s="2" t="n"/>
       <c r="L20" s="2" t="n">
+        <v>0.527</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>0.878</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>1289</v>
+      </c>
+      <c r="O20" s="2" t="n">
+        <v>443</v>
+      </c>
+      <c r="P20" s="2" t="n">
+        <v>1.611</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>Харківське ЛВУМГ</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>9.907</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>2831</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="F21" s="2" t="n"/>
+      <c r="G21" s="2" t="n">
+        <v>8.192</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>0.203</v>
+      </c>
+      <c r="J21" s="2" t="n"/>
+      <c r="K21" s="2" t="n"/>
+      <c r="L21" s="2" t="n">
         <v>0.8070000000000001</v>
       </c>
-      <c r="M20" s="2" t="n">
+      <c r="M21" s="2" t="n">
         <v>0.5800000000000001</v>
       </c>
-      <c r="N20" s="2" t="n">
+      <c r="N21" s="2" t="n">
         <v>2199</v>
       </c>
-      <c r="O20" s="2" t="n">
+      <c r="O21" s="2" t="n">
         <v>1041</v>
       </c>
-      <c r="P20" s="2" t="n">
+      <c r="P21" s="2" t="n">
         <v>3.305000000000001</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Check summ for distribution added
</commit_message>
<xml_diff>
--- a/Рознарядка.xlsx
+++ b/Рознарядка.xlsx
@@ -31927,7 +31927,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32946,6 +32946,69 @@
         <v>3.305000000000001</v>
       </c>
     </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Рознарядка. Контрольна сума:</t>
+        </is>
+      </c>
+      <c r="C23">
+        <f>SUM(C3:C21)</f>
+        <v/>
+      </c>
+      <c r="D23">
+        <f>SUM(D3:D21)</f>
+        <v/>
+      </c>
+      <c r="E23">
+        <f>SUM(E3:E21)</f>
+        <v/>
+      </c>
+      <c r="F23">
+        <f>SUM(F3:F21)</f>
+        <v/>
+      </c>
+      <c r="G23">
+        <f>SUM(G3:G21)</f>
+        <v/>
+      </c>
+      <c r="H23">
+        <f>SUM(H3:H21)</f>
+        <v/>
+      </c>
+      <c r="I23">
+        <f>SUM(I3:I21)</f>
+        <v/>
+      </c>
+      <c r="J23">
+        <f>SUM(J3:J21)</f>
+        <v/>
+      </c>
+      <c r="K23">
+        <f>SUM(K3:K21)</f>
+        <v/>
+      </c>
+      <c r="L23">
+        <f>SUM(L3:L21)</f>
+        <v/>
+      </c>
+      <c r="M23">
+        <f>SUM(M3:M21)</f>
+        <v/>
+      </c>
+      <c r="N23">
+        <f>SUM(N3:N21)</f>
+        <v/>
+      </c>
+      <c r="O23">
+        <f>SUM(O3:O21)</f>
+        <v/>
+      </c>
+      <c r="P23">
+        <f>SUM(P3:P21)</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:A2"/>

</xml_diff>